<commit_message>
The SRS issues were closed
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI\QA project Team D\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3722167-6AE2-464C-AB02-05C08403E2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="80">
   <si>
     <t>Review No.</t>
   </si>
@@ -281,11 +282,14 @@
   <si>
     <t>RMP_06</t>
   </si>
+  <si>
+    <t>26/4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
   </numFmts>
@@ -738,7 +742,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -788,7 +792,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
               </c:ext>
@@ -802,7 +806,7 @@
                 <a:srgbClr val="92D050"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
               </c:ext>
@@ -834,11 +838,13 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -866,11 +872,13 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -887,7 +895,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -912,7 +920,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -920,7 +928,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-27D6-487A-AA22-0D6B554A5A49}"/>
             </c:ext>
@@ -970,7 +978,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -992,7 +1000,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-03DF-44F1-832A-8EA9D7319E92}"/>
               </c:ext>
@@ -1006,7 +1014,7 @@
                 <a:srgbClr val="92D050"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-03DF-44F1-832A-8EA9D7319E92}"/>
               </c:ext>
@@ -1041,7 +1049,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-03DF-44F1-832A-8EA9D7319E92}"/>
             </c:ext>
@@ -1105,7 +1113,7 @@
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1136,7 +1144,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1575,7 +1583,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -1585,7 +1593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1682,7 +1690,7 @@
       </c>
       <c r="N3" s="24">
         <f>COUNTIFS(SRS!E2:E1047596,"Open")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
@@ -1758,7 +1766,7 @@
       </c>
       <c r="N5" s="24">
         <f>SUM(N3:N4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
@@ -29645,7 +29653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -29796,7 +29804,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -29805,7 +29813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -29939,7 +29947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30084,7 +30092,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30093,13 +30101,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -30240,7 +30248,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30249,7 +30257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30384,7 +30392,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30393,7 +30401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30527,7 +30535,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30536,12 +30544,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -30634,13 +30642,17 @@
         <v>62</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="37.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -30740,7 +30752,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30750,7 +30762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Update the review sheet
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8892AECC-E90C-4A7C-A5D4-D30C761F2BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421D484-E3D5-487C-AAEF-09C1AE0A904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
   <si>
     <t>Review No.</t>
   </si>
@@ -328,6 +330,9 @@
   </si>
   <si>
     <t>SRS_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update fuction names </t>
   </si>
 </sst>
 </file>
@@ -812,16 +817,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -846,6 +841,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,7 +1088,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1204,7 +1209,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1786,7 +1791,7 @@
       <c r="Z2" s="22"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="36" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -1804,7 +1809,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="M3" s="24" t="s">
@@ -1828,7 +1833,7 @@
       <c r="Z3" s="22"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="29"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="23" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +1849,7 @@
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
-      <c r="L4" s="32"/>
+      <c r="L4" s="40"/>
       <c r="M4" s="24" t="s">
         <v>58</v>
       </c>
@@ -1866,7 +1871,7 @@
       <c r="Z4" s="22"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="30"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="23" t="s">
         <v>59</v>
       </c>
@@ -1882,7 +1887,7 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="33"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="24" t="s">
         <v>59</v>
       </c>
@@ -30075,8 +30080,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -30160,15 +30165,27 @@
       <c r="A4" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="33.75" customHeight="1">
       <c r="A5" s="15" t="s">
@@ -30669,8 +30686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -30786,7 +30803,7 @@
       <c r="C5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>82</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -30806,7 +30823,7 @@
       <c r="C6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -30826,7 +30843,7 @@
       <c r="C7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -30837,44 +30854,44 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="72" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
       <c r="E10" s="13"/>

</xml_diff>

<commit_message>
add last updates on SRS and adding ERD
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI\QA project Team D\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8892AECC-E90C-4A7C-A5D4-D30C761F2BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="91">
   <si>
     <t>Review No.</t>
   </si>
@@ -316,12 +315,6 @@
     <t>SRS_07</t>
   </si>
   <si>
-    <t>Add Admin
-REQ-03-Add_Admin
-Does the admin will add a name or username ?
-As this will be contraductory requirment with requirment REQ-02-User_Login.</t>
-  </si>
-  <si>
     <t>Add Tour
 REQ-01-Add_Tour
 This requirement missed important information as flight date.</t>
@@ -329,11 +322,17 @@
   <si>
     <t>SRS_08</t>
   </si>
+  <si>
+    <t>Add Admin
+REQ-03-Add_Admin
+Does the admin will add a name or username ?
+As this will be contraductory requirment with requirment REQ-02-Admin_Login.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
   </numFmts>
@@ -812,16 +811,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -846,6 +835,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,7 +863,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -914,7 +913,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
               </c:ext>
@@ -928,7 +927,7 @@
                 <a:srgbClr val="92D050"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
               </c:ext>
@@ -960,13 +959,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -994,13 +991,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1017,7 +1012,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1050,7 +1045,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-27D6-487A-AA22-0D6B554A5A49}"/>
             </c:ext>
@@ -1083,7 +1078,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1100,7 +1095,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -1122,7 +1117,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-03DF-44F1-832A-8EA9D7319E92}"/>
               </c:ext>
@@ -1136,7 +1131,7 @@
                 <a:srgbClr val="92D050"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-03DF-44F1-832A-8EA9D7319E92}"/>
               </c:ext>
@@ -1171,7 +1166,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-03DF-44F1-832A-8EA9D7319E92}"/>
             </c:ext>
@@ -1204,7 +1199,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1235,7 +1230,7 @@
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1261,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1484,7 +1479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1705,7 +1700,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E20">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -1715,7 +1710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1786,7 +1781,7 @@
       <c r="Z2" s="22"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="36" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -1804,7 +1799,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="M3" s="24" t="s">
@@ -1828,7 +1823,7 @@
       <c r="Z3" s="22"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="29"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="23" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +1839,7 @@
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
-      <c r="L4" s="32"/>
+      <c r="L4" s="40"/>
       <c r="M4" s="24" t="s">
         <v>58</v>
       </c>
@@ -1866,7 +1861,7 @@
       <c r="Z4" s="22"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="30"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="23" t="s">
         <v>59</v>
       </c>
@@ -1882,7 +1877,7 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="33"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="24" t="s">
         <v>59</v>
       </c>
@@ -29775,7 +29770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -29926,7 +29921,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -29935,7 +29930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30069,7 +30064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30214,7 +30209,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30223,7 +30218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30370,7 +30365,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30379,7 +30374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30514,7 +30509,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30523,7 +30518,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30657,7 +30652,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30666,12 +30661,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -30786,13 +30781,15 @@
       <c r="C5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>82</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
@@ -30806,13 +30803,15 @@
       <c r="C6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="28" t="s">
         <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -30826,55 +30825,61 @@
       <c r="C7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="72" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" ht="45" customHeight="1">
+      <c r="A9" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-    </row>
-    <row r="9" spans="1:8" ht="45" customHeight="1">
-      <c r="A9" s="39" t="s">
-        <v>90</v>
+      <c r="F9" s="7" t="s">
+        <v>20</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
       <c r="E10" s="13"/>
@@ -30926,7 +30931,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E21">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -30936,7 +30941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Closed Issues found in SRS in Review sheet
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421D484-E3D5-487C-AAEF-09C1AE0A904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A2688F-EF79-45F1-923F-16FD2E0B9177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="92">
   <si>
     <t>Review No.</t>
   </si>
@@ -1047,7 +1045,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1088,7 +1086,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1209,7 +1207,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1817,7 +1815,7 @@
       </c>
       <c r="N3" s="24">
         <f>COUNTIFS(SRS!E2:E1047597,"Open")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
@@ -1893,7 +1891,7 @@
       </c>
       <c r="N5" s="24">
         <f>SUM(N3:N4)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
@@ -30080,7 +30078,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -30686,9 +30684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -30807,11 +30805,17 @@
         <v>82</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="49.8" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -30827,11 +30831,17 @@
         <v>83</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="60.6" customHeight="1">
       <c r="A7" s="5" t="s">
@@ -30847,11 +30857,17 @@
         <v>84</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="F7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="72" customHeight="1">
       <c r="A8" s="29" t="s">
@@ -30867,11 +30883,17 @@
         <v>88</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
+      <c r="F8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1">
       <c r="A9" s="33" t="s">
@@ -30887,11 +30909,17 @@
         <v>89</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
+      <c r="F9" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
       <c r="E10" s="13"/>

</xml_diff>

<commit_message>
updating reviews and RTm
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\QA Project\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391FB71-4B78-4F9D-BCD4-3197AC0993BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
   <si>
     <t>Review No.</t>
   </si>
@@ -464,11 +463,32 @@
 8. Home for the user is missed as Layout.
 </t>
   </si>
+  <si>
+    <t>TB_03</t>
+  </si>
+  <si>
+    <t>SIQ_11_Tour is repated twice at Customer_Requirement_04</t>
+  </si>
+  <si>
+    <t>08/5</t>
+  </si>
+  <si>
+    <t>TB_04</t>
+  </si>
+  <si>
+    <t>TB_05</t>
+  </si>
+  <si>
+    <t>Feedback removing is not applied at Customer_Requirement_05</t>
+  </si>
+  <si>
+    <t>SIQ_06_Add_User  is not related to  Customer_Requirement_09</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
   </numFmts>
@@ -589,7 +609,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -982,11 +1002,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1220,6 +1251,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,9 +1375,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
@@ -1369,9 +1407,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
@@ -1457,7 +1493,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1578,7 +1614,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1858,7 +1894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1866,15 +1902,15 @@
       <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" customHeight="1">
@@ -2372,7 +2408,7 @@
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E24">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -2382,20 +2418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693EB218-C1D8-4EEC-B91D-4737533220EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="41.4" customHeight="1">
+    <row r="2" spans="1:8" ht="41.45" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>102</v>
       </c>
@@ -2491,7 +2527,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{CB32F748-C54E-4EDD-A87E-0460FE4D6BA9}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -2500,14 +2536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="14.25" customHeight="1">
@@ -3525,20 +3561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="12" width="8.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -31587,20 +31623,20 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB107C2-CBBE-4F90-A398-7916335DFE6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31648,7 +31684,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9" ht="57.6">
+    <row r="3" spans="1:9" ht="60">
       <c r="A3" s="46" t="s">
         <v>98</v>
       </c>
@@ -31721,7 +31757,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{E7E5512A-606D-4770-9933-CD648ADE2F36}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -31730,20 +31766,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891C4D3F-DDC9-49C8-96F1-9961B200D3E7}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31769,7 +31805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.8" customHeight="1">
+    <row r="2" spans="1:8" ht="31.9" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -31789,7 +31825,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:8" ht="31.8" customHeight="1">
+    <row r="3" spans="1:8" ht="31.9" customHeight="1">
       <c r="A3" s="46" t="s">
         <v>106</v>
       </c>
@@ -31808,56 +31844,123 @@
       <c r="F3" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="52" t="s">
-        <v>109</v>
+      <c r="G3" s="55" t="s">
+        <v>131</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="46"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>130</v>
+      </c>
       <c r="E4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="F4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{6396AF7A-EFEF-4F01-8DB0-266011A077AE}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E6">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3753E40-BA73-4C99-A3AD-7F839E90F709}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="29"/>
-    <col min="4" max="4" width="20.6640625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="29" customWidth="1"/>
+    <col min="1" max="3" width="8.85546875" style="29"/>
+    <col min="4" max="4" width="20.7109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="29" customWidth="1"/>
     <col min="6" max="6" width="10" style="29" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="29" customWidth="1"/>
-    <col min="8" max="17" width="8.88671875" style="29"/>
-    <col min="18" max="19" width="8.88671875" style="29" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="29"/>
+    <col min="7" max="7" width="13.85546875" style="29" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" style="29"/>
+    <col min="18" max="19" width="8.85546875" style="29" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -31885,7 +31988,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1">
+    <row r="2" spans="1:10" ht="34.15" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>84</v>
       </c>
@@ -31913,7 +32016,7 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1">
+    <row r="3" spans="1:10" ht="29.45" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -31925,7 +32028,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:10" ht="29.4" customHeight="1">
+    <row r="4" spans="1:10" ht="29.45" customHeight="1">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -31937,7 +32040,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="29.4" customHeight="1">
+    <row r="5" spans="1:10" ht="29.45" customHeight="1">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -31949,7 +32052,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="28.2" customHeight="1">
+    <row r="6" spans="1:10" ht="28.15" customHeight="1">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -31988,7 +32091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -31998,12 +32101,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32055,7 +32158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8">
       <c r="A3" s="44" t="s">
         <v>92</v>
       </c>
@@ -32075,7 +32178,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8">
       <c r="A4" s="44" t="s">
         <v>93</v>
       </c>
@@ -32095,7 +32198,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="43.2">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="44" t="s">
         <v>94</v>
       </c>
@@ -32121,7 +32224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
+    <row r="6" spans="1:8">
       <c r="A6" s="44" t="s">
         <v>95</v>
       </c>
@@ -32135,7 +32238,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="45" t="s">
         <v>96</v>
       </c>
@@ -32151,7 +32254,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32160,7 +32263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32170,9 +32273,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1">
@@ -32308,7 +32411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32318,12 +32421,12 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32465,7 +32568,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32474,7 +32577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32484,12 +32587,12 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32567,7 +32670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" customHeight="1">
+    <row r="4" spans="1:8" ht="43.15" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -32593,7 +32696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.2" customHeight="1">
+    <row r="5" spans="1:8" ht="409.15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
@@ -32645,7 +32748,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32654,7 +32757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32664,14 +32767,14 @@
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32697,7 +32800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -32789,7 +32892,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32798,7 +32901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32808,13 +32911,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32840,7 +32943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
@@ -32932,7 +33035,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32941,21 +33044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1">
@@ -33113,7 +33216,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" customHeight="1">
+    <row r="8" spans="1:9" ht="86.45" customHeight="1">
       <c r="A8" s="26" t="s">
         <v>69</v>
       </c>
@@ -33140,7 +33243,7 @@
       </c>
       <c r="I8" s="60"/>
     </row>
-    <row r="9" spans="1:9" ht="49.8" customHeight="1">
+    <row r="9" spans="1:9" ht="49.9" customHeight="1">
       <c r="A9" s="26" t="s">
         <v>73</v>
       </c>
@@ -33221,7 +33324,7 @@
       </c>
       <c r="I11" s="60"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2">
+    <row r="12" spans="1:9" ht="45">
       <c r="A12" s="26" t="s">
         <v>78</v>
       </c>
@@ -33248,7 +33351,7 @@
       </c>
       <c r="I12" s="60"/>
     </row>
-    <row r="13" spans="1:9" ht="28.2" customHeight="1">
+    <row r="13" spans="1:9" ht="28.15" customHeight="1">
       <c r="A13" s="80" t="s">
         <v>115</v>
       </c>
@@ -33263,7 +33366,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="26" t="s">
         <v>99</v>
       </c>
@@ -33303,7 +33406,7 @@
       <c r="H15" s="82"/>
       <c r="I15" s="60"/>
     </row>
-    <row r="16" spans="1:9" ht="28.2" customHeight="1">
+    <row r="16" spans="1:9" ht="28.15" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>118</v>
       </c>
@@ -33373,7 +33476,7 @@
     <mergeCell ref="A15:H15"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
adding low level flowcharts after updating
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\QA Project\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5391FB71-4B78-4F9D-BCD4-3197AC0993BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
   <si>
     <t>Review No.</t>
   </si>
@@ -464,11 +463,32 @@
 8. Home for the user is missed as Layout.
 </t>
   </si>
+  <si>
+    <t>TB_03</t>
+  </si>
+  <si>
+    <t>SIQ_11_Tour is repated twice at Customer_Requirement_04</t>
+  </si>
+  <si>
+    <t>08/5</t>
+  </si>
+  <si>
+    <t>TB_04</t>
+  </si>
+  <si>
+    <t>TB_05</t>
+  </si>
+  <si>
+    <t>Feedback removing is not applied at Customer_Requirement_05</t>
+  </si>
+  <si>
+    <t>SIQ_06_Add_User  is not related to  Customer_Requirement_09</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
   </numFmts>
@@ -589,7 +609,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -982,11 +1002,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1220,6 +1251,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,9 +1375,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
@@ -1369,9 +1407,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:showDataLabelsRange val="0"/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-27D6-487A-AA22-0D6B554A5A49}"/>
                 </c:ext>
@@ -1457,7 +1493,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1578,7 +1614,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1858,7 +1894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1866,15 +1902,15 @@
       <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" customHeight="1">
@@ -2372,7 +2408,7 @@
     <mergeCell ref="A10:H10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E24">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -2382,20 +2418,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693EB218-C1D8-4EEC-B91D-4737533220EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="41.4" customHeight="1">
+    <row r="2" spans="1:8" ht="41.45" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>102</v>
       </c>
@@ -2491,7 +2527,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{CB32F748-C54E-4EDD-A87E-0460FE4D6BA9}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -2500,14 +2536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="14.25" customHeight="1">
@@ -3525,20 +3561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="12" width="8.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -31587,20 +31623,20 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB107C2-CBBE-4F90-A398-7916335DFE6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31648,7 +31684,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9" ht="57.6">
+    <row r="3" spans="1:9" ht="60">
       <c r="A3" s="46" t="s">
         <v>98</v>
       </c>
@@ -31721,7 +31757,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{E7E5512A-606D-4770-9933-CD648ADE2F36}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -31730,20 +31766,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891C4D3F-DDC9-49C8-96F1-9961B200D3E7}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31769,7 +31805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.8" customHeight="1">
+    <row r="2" spans="1:8" ht="31.9" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -31789,7 +31825,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:8" ht="31.8" customHeight="1">
+    <row r="3" spans="1:8" ht="31.9" customHeight="1">
       <c r="A3" s="46" t="s">
         <v>106</v>
       </c>
@@ -31808,56 +31844,123 @@
       <c r="F3" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="52" t="s">
-        <v>109</v>
+      <c r="G3" s="55" t="s">
+        <v>131</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="46"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>130</v>
+      </c>
       <c r="E4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="F4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="89">
+        <v>44690</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="90">
+        <v>44690</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{6396AF7A-EFEF-4F01-8DB0-266011A077AE}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E6">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3753E40-BA73-4C99-A3AD-7F839E90F709}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="29"/>
-    <col min="4" max="4" width="20.6640625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="29" customWidth="1"/>
+    <col min="1" max="3" width="8.85546875" style="29"/>
+    <col min="4" max="4" width="20.7109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="29" customWidth="1"/>
     <col min="6" max="6" width="10" style="29" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="29" customWidth="1"/>
-    <col min="8" max="17" width="8.88671875" style="29"/>
-    <col min="18" max="19" width="8.88671875" style="29" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="29"/>
+    <col min="7" max="7" width="13.85546875" style="29" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" style="29"/>
+    <col min="18" max="19" width="8.85546875" style="29" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -31885,7 +31988,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1">
+    <row r="2" spans="1:10" ht="34.15" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>84</v>
       </c>
@@ -31913,7 +32016,7 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1">
+    <row r="3" spans="1:10" ht="29.45" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -31925,7 +32028,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:10" ht="29.4" customHeight="1">
+    <row r="4" spans="1:10" ht="29.45" customHeight="1">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -31937,7 +32040,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="29.4" customHeight="1">
+    <row r="5" spans="1:10" ht="29.45" customHeight="1">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -31949,7 +32052,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="28.2" customHeight="1">
+    <row r="6" spans="1:10" ht="28.15" customHeight="1">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -31988,7 +32091,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -31998,12 +32101,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32055,7 +32158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8">
       <c r="A3" s="44" t="s">
         <v>92</v>
       </c>
@@ -32075,7 +32178,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8">
       <c r="A4" s="44" t="s">
         <v>93</v>
       </c>
@@ -32095,7 +32198,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="43.2">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="44" t="s">
         <v>94</v>
       </c>
@@ -32121,7 +32224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
+    <row r="6" spans="1:8">
       <c r="A6" s="44" t="s">
         <v>95</v>
       </c>
@@ -32135,7 +32238,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="45" t="s">
         <v>96</v>
       </c>
@@ -32151,7 +32254,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32160,7 +32263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32170,9 +32273,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1">
@@ -32308,7 +32411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32318,12 +32421,12 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32465,7 +32568,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32474,7 +32577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32484,12 +32587,12 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32567,7 +32670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" customHeight="1">
+    <row r="4" spans="1:8" ht="43.15" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -32593,7 +32696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.2" customHeight="1">
+    <row r="5" spans="1:8" ht="409.15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
@@ -32645,7 +32748,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32654,7 +32757,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32664,14 +32767,14 @@
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32697,7 +32800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -32789,7 +32892,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32798,7 +32901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32808,13 +32911,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32840,7 +32943,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
@@ -32932,7 +33035,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -32941,21 +33044,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1">
@@ -33113,7 +33216,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" customHeight="1">
+    <row r="8" spans="1:9" ht="86.45" customHeight="1">
       <c r="A8" s="26" t="s">
         <v>69</v>
       </c>
@@ -33140,7 +33243,7 @@
       </c>
       <c r="I8" s="60"/>
     </row>
-    <row r="9" spans="1:9" ht="49.8" customHeight="1">
+    <row r="9" spans="1:9" ht="49.9" customHeight="1">
       <c r="A9" s="26" t="s">
         <v>73</v>
       </c>
@@ -33221,7 +33324,7 @@
       </c>
       <c r="I11" s="60"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2">
+    <row r="12" spans="1:9" ht="45">
       <c r="A12" s="26" t="s">
         <v>78</v>
       </c>
@@ -33248,7 +33351,7 @@
       </c>
       <c r="I12" s="60"/>
     </row>
-    <row r="13" spans="1:9" ht="28.2" customHeight="1">
+    <row r="13" spans="1:9" ht="28.15" customHeight="1">
       <c r="A13" s="80" t="s">
         <v>115</v>
       </c>
@@ -33263,7 +33366,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="26" t="s">
         <v>99</v>
       </c>
@@ -33303,7 +33406,7 @@
       <c r="H15" s="82"/>
       <c r="I15" s="60"/>
     </row>
-    <row r="16" spans="1:9" ht="28.2" customHeight="1">
+    <row r="16" spans="1:9" ht="28.15" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>118</v>
       </c>
@@ -33373,7 +33476,7 @@
     <mergeCell ref="A15:H15"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Upload TravelAdvisorProject V1.0 whith update in PMP [File structure] & database comments in DB
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0E8B2-94A4-4E82-9EB2-A9398B5E4ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6E8D5F-AE94-4687-A47F-4984B208AD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,17 @@
     <sheet name="Scope Statment" sheetId="13" r:id="rId13"/>
     <sheet name="Tracability" sheetId="16" r:id="rId14"/>
     <sheet name="Issue managment" sheetId="17" r:id="rId15"/>
+    <sheet name="DataBase" sheetId="18" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="141">
   <si>
     <t>Review No.</t>
   </si>
@@ -494,6 +493,15 @@
   <si>
     <t>Update esclation</t>
   </si>
+  <si>
+    <t>DB_01</t>
+  </si>
+  <si>
+    <t>Osama</t>
+  </si>
+  <si>
+    <t>Data types in database is not valid</t>
+  </si>
 </sst>
 </file>
 
@@ -619,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1012,22 +1020,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1242,7 +1239,25 @@
     <xf numFmtId="16" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1916,15 +1931,15 @@
       <selection pane="bottomLeft" activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" customHeight="1">
@@ -1975,16 +1990,16 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
@@ -2125,18 +2140,18 @@
       <c r="AA5" s="61"/>
     </row>
     <row r="6" spans="1:27" ht="37.5" customHeight="1">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
       <c r="K6" s="60"/>
@@ -2205,16 +2220,16 @@
       <c r="AA7" s="61"/>
     </row>
     <row r="8" spans="1:27" ht="37.5" customHeight="1">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
       <c r="K8" s="60"/>
@@ -2283,16 +2298,16 @@
       <c r="AA9" s="61"/>
     </row>
     <row r="10" spans="1:27" ht="37.5" customHeight="1">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
       <c r="I10" s="60"/>
       <c r="J10" s="60"/>
       <c r="K10" s="60"/>
@@ -2361,16 +2376,16 @@
       <c r="AA11" s="61"/>
     </row>
     <row r="12" spans="1:27" ht="37.5" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
       <c r="I12" s="60"/>
       <c r="J12" s="60"/>
       <c r="K12" s="60"/>
@@ -2508,13 +2523,13 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2555,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="41.4" customHeight="1">
+    <row r="2" spans="1:8" ht="41.45" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>102</v>
       </c>
@@ -2624,9 +2639,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="14.25" customHeight="1">
@@ -3648,16 +3663,16 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="12" width="8.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3717,7 +3732,7 @@
       <c r="Z2" s="19"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="92" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -3735,7 +3750,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="89" t="s">
+      <c r="L3" s="95" t="s">
         <v>45</v>
       </c>
       <c r="M3" s="21" t="s">
@@ -3759,7 +3774,7 @@
       <c r="Z3" s="19"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="87"/>
+      <c r="A4" s="93"/>
       <c r="B4" s="20" t="s">
         <v>46</v>
       </c>
@@ -3775,7 +3790,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
-      <c r="L4" s="90"/>
+      <c r="L4" s="96"/>
       <c r="M4" s="21" t="s">
         <v>46</v>
       </c>
@@ -3797,7 +3812,7 @@
       <c r="Z4" s="19"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="88"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="20" t="s">
         <v>47</v>
       </c>
@@ -3813,7 +3828,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
-      <c r="L5" s="91"/>
+      <c r="L5" s="97"/>
       <c r="M5" s="21" t="s">
         <v>47</v>
       </c>
@@ -31710,16 +31725,16 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31767,7 +31782,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9" ht="57.6">
+    <row r="3" spans="1:9" ht="60">
       <c r="A3" s="46" t="s">
         <v>98</v>
       </c>
@@ -31853,162 +31868,162 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" ht="30">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="80" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.95" customHeight="1">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:8" ht="31.9" customHeight="1">
+      <c r="A2" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="1:8" ht="31.95" customHeight="1">
-      <c r="A3" s="46" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+    </row>
+    <row r="3" spans="1:8" ht="31.9" customHeight="1">
+      <c r="A3" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="84" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="85">
         <v>44690</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="85">
         <v>44690</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="84" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="85">
         <v>44690</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="79">
+      <c r="G5" s="85">
         <v>44690</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="84" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8">
-      <c r="A6" s="46" t="s">
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="85">
         <v>44690</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="79">
+      <c r="G6" s="85">
         <v>44690</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="84" t="s">
         <v>10</v>
       </c>
     </row>
@@ -32028,16 +32043,16 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8">
+    <row r="1" spans="1:8" ht="30">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -32063,7 +32078,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.95" customHeight="1">
+    <row r="2" spans="1:8" ht="31.9" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -32089,7 +32104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="31.95" customHeight="1">
+    <row r="3" spans="1:8" ht="31.9" customHeight="1">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="53"/>
@@ -32120,6 +32135,108 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D011AC19-4C52-43BF-AEA4-719A8F1801E3}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="50.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="48">
+        <v>44692</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="35">
+        <v>44692</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="49"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="46"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="49"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{C0687E38-DDE0-4530-B22D-9FFF83BFE362}">
+      <formula1>Options</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
@@ -32128,19 +32245,19 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="29"/>
-    <col min="4" max="4" width="20.6640625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="29" customWidth="1"/>
+    <col min="1" max="3" width="8.85546875" style="29"/>
+    <col min="4" max="4" width="20.7109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="29" customWidth="1"/>
     <col min="6" max="6" width="10" style="29" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="29" customWidth="1"/>
-    <col min="8" max="17" width="8.88671875" style="29"/>
-    <col min="18" max="19" width="8.88671875" style="29" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="29"/>
+    <col min="7" max="7" width="13.85546875" style="29" customWidth="1"/>
+    <col min="8" max="17" width="8.85546875" style="29"/>
+    <col min="18" max="19" width="8.85546875" style="29" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -32168,7 +32285,7 @@
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1">
+    <row r="2" spans="1:10" ht="34.15" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>84</v>
       </c>
@@ -32196,7 +32313,7 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="1:10" ht="29.4" customHeight="1">
+    <row r="3" spans="1:10" ht="29.45" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -32208,7 +32325,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:10" ht="29.4" customHeight="1">
+    <row r="4" spans="1:10" ht="29.45" customHeight="1">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -32220,7 +32337,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="29.4" customHeight="1">
+    <row r="5" spans="1:10" ht="29.45" customHeight="1">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -32232,7 +32349,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="28.2" customHeight="1">
+    <row r="6" spans="1:10" ht="28.15" customHeight="1">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -32281,12 +32398,12 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32338,7 +32455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8">
       <c r="A3" s="44" t="s">
         <v>92</v>
       </c>
@@ -32358,7 +32475,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8">
       <c r="A4" s="44" t="s">
         <v>93</v>
       </c>
@@ -32378,7 +32495,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="43.2">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="44" t="s">
         <v>94</v>
       </c>
@@ -32404,7 +32521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
+    <row r="6" spans="1:8">
       <c r="A6" s="44" t="s">
         <v>95</v>
       </c>
@@ -32418,7 +32535,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" thickBot="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
       <c r="A7" s="45" t="s">
         <v>96</v>
       </c>
@@ -32453,9 +32570,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1">
@@ -32601,12 +32718,12 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32767,12 +32884,12 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32850,7 +32967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" customHeight="1">
+    <row r="4" spans="1:8" ht="43.15" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
@@ -32876,7 +32993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.2" customHeight="1">
+    <row r="5" spans="1:8" ht="409.15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>37</v>
       </c>
@@ -32947,14 +33064,14 @@
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32980,7 +33097,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
@@ -33091,13 +33208,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -33123,7 +33240,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="12" t="s">
         <v>61</v>
       </c>
@@ -33231,14 +33348,14 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="64.44140625" customWidth="1"/>
-    <col min="5" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" customWidth="1"/>
+    <col min="5" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1">
@@ -33380,23 +33497,23 @@
       <c r="I6" s="60"/>
     </row>
     <row r="7" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84" t="s">
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="85"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91"/>
       <c r="I7" s="60" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" customHeight="1">
+    <row r="8" spans="1:9" ht="86.45" customHeight="1">
       <c r="A8" s="26" t="s">
         <v>69</v>
       </c>
@@ -33423,7 +33540,7 @@
       </c>
       <c r="I8" s="60"/>
     </row>
-    <row r="9" spans="1:9" ht="49.95" customHeight="1">
+    <row r="9" spans="1:9" ht="49.9" customHeight="1">
       <c r="A9" s="26" t="s">
         <v>73</v>
       </c>
@@ -33504,7 +33621,7 @@
       </c>
       <c r="I11" s="60"/>
     </row>
-    <row r="12" spans="1:9" ht="43.2">
+    <row r="12" spans="1:9" ht="45">
       <c r="A12" s="26" t="s">
         <v>78</v>
       </c>
@@ -33531,22 +33648,22 @@
       </c>
       <c r="I12" s="60"/>
     </row>
-    <row r="13" spans="1:9" ht="28.2" customHeight="1">
-      <c r="A13" s="83" t="s">
+    <row r="13" spans="1:9" ht="28.15" customHeight="1">
+      <c r="A13" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="85"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="91"/>
       <c r="I13" s="60" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.8">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="26" t="s">
         <v>99</v>
       </c>
@@ -33574,19 +33691,19 @@
       <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:9" ht="33" customHeight="1">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="85"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="91"/>
       <c r="I15" s="60"/>
     </row>
-    <row r="16" spans="1:9" ht="28.2" customHeight="1">
+    <row r="16" spans="1:9" ht="28.15" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Update low level designs, Update Review Sheet , Upload Issue Log
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6E8D5F-AE94-4687-A47F-4984B208AD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F55A915-F94C-4E55-AA6A-AE073DC34370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
   <definedNames>
     <definedName name="Options">Options!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="152">
   <si>
     <t>Review No.</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>ERD_04</t>
-  </si>
-  <si>
-    <t>ERD_05</t>
   </si>
   <si>
     <t>ERD_06</t>
@@ -433,11 +430,6 @@
  is redudant.</t>
   </si>
   <si>
-    <t>In admin entity, name of the admin should be username,
-In User entity, username is missed.
-In Tour entity, start date should be end date.</t>
-  </si>
-  <si>
     <t>Aya  Ahmed</t>
   </si>
   <si>
@@ -451,20 +443,6 @@
   </si>
   <si>
     <t>All dates in constraints assigned in the time section are not correct.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.  About us in the navigation bar is missed in 
-Layout_Add_Admin
-Layout_Add_Tour
-Layout_Add_User
-2. The name in the Layout_Add_Admin should be username
-3. Tour name is written wrong, Flight_Date is missed, end date is missed, Duration,  in the Layout_Add_Tour, Button should be added only.
-4. About us button in Tour 1 is redundant as it is already in the navigation bar. 
-5. Start date should bd end date.
-6. The rating is missed in Tour1 where user can insert his rating.
-7. Home is missed in the navigation bar in Home in layout_Home.
-8. Home for the user is missed as Layout.
-</t>
   </si>
   <si>
     <t>TB_03</t>
@@ -501,6 +479,64 @@
   </si>
   <si>
     <t>Data types in database is not valid</t>
+  </si>
+  <si>
+    <t>low-level designs weren't accurate enough.</t>
+  </si>
+  <si>
+    <t>12/5</t>
+  </si>
+  <si>
+    <t>the if-else should be in two blocks , 
+db wasn't should be in the digram.</t>
+  </si>
+  <si>
+    <t>10/5</t>
+  </si>
+  <si>
+    <t>13/5</t>
+  </si>
+  <si>
+    <t>In admin entity, name of the admin should be username,
+In User entity, username is missed.
+In Tour entity, start date should be end date.
+The relation between tour, and the user should be 1 to many.</t>
+  </si>
+  <si>
+    <t>Remove feedback, rating functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  About us in the navigation bar is missed in 
+Layout_Add_Admin
+Layout_Add_Tour
+Layout_Add_User
+2. The name in the Layout_Add_Admin should be username
+3. Tour name is written wrong, Flight_Date is missed, end date is missed, Duration,  in the Layout_Add_Tour, Button should be added only.
+4. About us button in Tour 1 is redundant as it is already in the navigation bar. 
+5. Start date should bd end date.
+6. Home is missed in the navigation bar in Home in layout_Home.
+7. Home for the user is missed as Layout.
+</t>
+  </si>
+  <si>
+    <t>Remove video, rating, and feedback from Layout_Tour, Layout_Add_Tour
+Instead in Layout_Add_Tour remove video and inset picture.</t>
+  </si>
+  <si>
+    <t>SRS_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating functional requirments
+</t>
+  </si>
+  <si>
+    <t>Version 1.5</t>
+  </si>
+  <si>
+    <t>Updating project schedule</t>
+  </si>
+  <si>
+    <t>11/5</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1285,6 +1321,22 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1522,7 +1574,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1643,7 +1695,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1927,19 +1979,19 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB12" sqref="AB12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" customWidth="1"/>
-    <col min="5" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="64.44140625" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" customHeight="1">
@@ -1959,13 +2011,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
@@ -1986,12 +2038,12 @@
       <c r="Y1" s="26"/>
       <c r="Z1" s="26"/>
       <c r="AA1" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1">
       <c r="A2" s="87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88"/>
@@ -2019,12 +2071,12 @@
       <c r="Y2" s="26"/>
       <c r="Z2" s="26"/>
       <c r="AA2" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="37.5" customHeight="1">
       <c r="A3" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>6</v>
@@ -2063,7 +2115,7 @@
     </row>
     <row r="4" spans="1:27" ht="37.5" customHeight="1">
       <c r="A4" s="50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>10</v>
@@ -2102,7 +2154,7 @@
     </row>
     <row r="5" spans="1:27" ht="37.5" customHeight="1">
       <c r="A5" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>12</v>
@@ -2141,12 +2193,12 @@
     </row>
     <row r="6" spans="1:27" ht="37.5" customHeight="1">
       <c r="A6" s="87" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="88"/>
       <c r="C6" s="88"/>
       <c r="D6" s="88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="88"/>
       <c r="F6" s="88"/>
@@ -2171,21 +2223,21 @@
       <c r="Y6" s="60"/>
       <c r="Z6" s="60"/>
       <c r="AA6" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="37.5" customHeight="1">
       <c r="A7" s="50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="26" t="s">
         <v>9</v>
@@ -2194,7 +2246,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>10</v>
@@ -2221,7 +2273,7 @@
     </row>
     <row r="8" spans="1:27" ht="37.5" customHeight="1">
       <c r="A8" s="87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
@@ -2249,21 +2301,21 @@
       <c r="Y8" s="60"/>
       <c r="Z8" s="60"/>
       <c r="AA8" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="37.5" customHeight="1">
       <c r="A9" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>9</v>
@@ -2272,7 +2324,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>12</v>
@@ -2299,7 +2351,7 @@
     </row>
     <row r="10" spans="1:27" ht="37.5" customHeight="1">
       <c r="A10" s="87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -2327,21 +2379,21 @@
       <c r="Y10" s="60"/>
       <c r="Z10" s="60"/>
       <c r="AA10" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="37.5" customHeight="1">
       <c r="A11" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="50" t="s">
         <v>9</v>
@@ -2350,7 +2402,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="63" t="s">
         <v>18</v>
@@ -2377,7 +2429,7 @@
     </row>
     <row r="12" spans="1:27" ht="37.5" customHeight="1">
       <c r="A12" s="87" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -2405,33 +2457,33 @@
       <c r="Y12" s="60"/>
       <c r="Z12" s="60"/>
       <c r="AA12" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="37.5" customHeight="1">
       <c r="A13" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="E13" s="50" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="50" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G13" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="63" t="s">
         <v>136</v>
-      </c>
-      <c r="H13" s="63" t="s">
-        <v>10</v>
       </c>
       <c r="I13" s="60"/>
       <c r="J13" s="60"/>
@@ -2453,17 +2505,112 @@
       <c r="Z13" s="60"/>
       <c r="AA13" s="61"/>
     </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1">
-      <c r="E14" s="10"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1">
-      <c r="E15" s="10"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1">
-      <c r="E16" s="10"/>
-      <c r="G16" s="11"/>
+    <row r="14" spans="1:27" ht="34.799999999999997" customHeight="1">
+      <c r="A14" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="61"/>
+    </row>
+    <row r="15" spans="1:27" ht="39.6" customHeight="1">
+      <c r="A15" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="60"/>
+      <c r="AA15" s="59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="37.200000000000003" customHeight="1">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60"/>
+      <c r="X16" s="60"/>
+      <c r="Y16" s="60"/>
+      <c r="Z16" s="60"/>
+      <c r="AA16" s="61"/>
     </row>
     <row r="17" spans="5:7" ht="14.25" customHeight="1">
       <c r="E17" s="10"/>
@@ -2498,7 +2645,8 @@
       <c r="G24" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A8:H8"/>
@@ -2506,7 +2654,7 @@
     <mergeCell ref="A12:H12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E16:E24 E3:E15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>
@@ -2523,13 +2671,13 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2546,24 +2694,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="41.45" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="41.4" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>16</v>
@@ -2577,28 +2725,28 @@
     </row>
     <row r="3" spans="1:8" ht="39.6" customHeight="1">
       <c r="A3" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="47" t="s">
         <v>103</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>104</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2639,14 +2787,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="14.25" customHeight="1">
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="14.25" customHeight="1">
@@ -3666,13 +3814,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="12" width="8.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3733,10 +3881,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="20">
         <f>COUNTIFS(PMP!E3:E1047600,"Open")</f>
@@ -3751,10 +3899,10 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N3" s="21">
         <f>COUNTIFS(SRS!E3:E1047602,"Open")</f>
@@ -3776,7 +3924,7 @@
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="93"/>
       <c r="B4" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="20">
         <f>COUNTIFS(PMP!E3:E1047600,"Closed")</f>
@@ -3792,7 +3940,7 @@
       <c r="K4" s="18"/>
       <c r="L4" s="96"/>
       <c r="M4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" s="21">
         <f>COUNTIFS(SRS!E3:E1047602,"Closed")</f>
@@ -3814,7 +3962,7 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="94"/>
       <c r="B5" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="20">
         <f>SUM(C3:C4)</f>
@@ -3830,7 +3978,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="97"/>
       <c r="M5" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="21">
         <f>SUM(N3:N4)</f>
@@ -31728,13 +31876,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="28.8">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -31751,19 +31899,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>10</v>
@@ -31782,18 +31930,18 @@
       <c r="H2" s="35"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9" ht="60">
+    <row r="3" spans="1:9" ht="57.6">
       <c r="A3" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>9</v>
@@ -31802,7 +31950,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>18</v>
@@ -31871,13 +32019,13 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="43.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
@@ -31894,24 +32042,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="80" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="31.9" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" customHeight="1">
       <c r="A2" s="67" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="67" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="67" t="s">
         <v>16</v>
@@ -31923,50 +32071,50 @@
       <c r="G2" s="82"/>
       <c r="H2" s="82"/>
     </row>
-    <row r="3" spans="1:8" ht="31.9" customHeight="1">
+    <row r="3" spans="1:8" ht="51.6" customHeight="1">
       <c r="A3" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="67" t="s">
         <v>106</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>107</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="83" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H3" s="84" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="55.2" customHeight="1">
       <c r="A4" s="67" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="85">
         <v>44690</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E4" s="67" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="85">
         <v>44690</v>
@@ -31975,24 +32123,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="44.4" customHeight="1">
       <c r="A5" s="67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="85">
         <v>44690</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E5" s="67" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="85">
         <v>44690</v>
@@ -32001,24 +32149,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="48.6" customHeight="1">
       <c r="A6" s="67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="85">
         <v>44690</v>
       </c>
       <c r="D6" s="86" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="67" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="85">
         <v>44690</v>
@@ -32042,17 +32190,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04B1DF2-7CE8-4C79-ACD7-56C61304D32C}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="43.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -32069,27 +32217,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="31.9" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="31.95" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="48">
         <v>44689</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>9</v>
@@ -32104,7 +32252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="31.9" customHeight="1">
+    <row r="3" spans="1:8" ht="31.95" customHeight="1">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="53"/>
@@ -32143,19 +32291,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="28.8">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -32172,27 +32320,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="50.25" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" s="48">
         <v>44692</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>9</v>
@@ -32245,19 +32393,19 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="29"/>
-    <col min="4" max="4" width="20.7109375" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="29" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="29"/>
+    <col min="4" max="4" width="20.6640625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="29" customWidth="1"/>
     <col min="6" max="6" width="10" style="29" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="29" customWidth="1"/>
-    <col min="8" max="17" width="8.85546875" style="29"/>
-    <col min="18" max="19" width="8.85546875" style="29" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="29"/>
+    <col min="7" max="7" width="13.88671875" style="29" customWidth="1"/>
+    <col min="8" max="17" width="8.88671875" style="29"/>
+    <col min="18" max="19" width="8.88671875" style="29" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="28.8">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -32274,38 +32422,38 @@
         <v>4</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="39" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
     </row>
-    <row r="2" spans="1:10" ht="34.15" customHeight="1">
+    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H2" s="42" t="s">
         <v>18</v>
@@ -32313,7 +32461,7 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="1:10" ht="29.45" customHeight="1">
+    <row r="3" spans="1:10" ht="29.4" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -32325,7 +32473,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:10" ht="29.45" customHeight="1">
+    <row r="4" spans="1:10" ht="29.4" customHeight="1">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -32337,7 +32485,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="5" spans="1:10" ht="29.45" customHeight="1">
+    <row r="5" spans="1:10" ht="29.4" customHeight="1">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -32349,7 +32497,7 @@
       <c r="I5" s="36"/>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10" ht="28.15" customHeight="1">
+    <row r="6" spans="1:10" ht="28.2" customHeight="1">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -32395,22 +32543,24 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="101"/>
+    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="101"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="103" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -32420,23 +32570,23 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="99" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="57" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="77" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -32446,23 +32596,23 @@
         <v>9</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="98" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="40.200000000000003" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="77" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -32472,17 +32622,17 @@
         <v>9</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="98"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="39" customHeight="1">
       <c r="A4" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="77" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -32492,21 +32642,21 @@
         <v>9</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="98"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="45">
+    <row r="5" spans="1:8" ht="43.2">
       <c r="A5" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="68" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>9</v>
@@ -32515,39 +32665,63 @@
         <v>18</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H5" s="70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="39.6" customHeight="1">
       <c r="A6" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="98" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="41.4" customHeight="1" thickBot="1">
       <c r="A7" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="100" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>140</v>
+      </c>
       <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -32564,15 +32738,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="61.7109375" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="101"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1">
@@ -32589,13 +32764,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="99" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30.75" customHeight="1">
@@ -32614,7 +32789,7 @@
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="98" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -32635,7 +32810,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="98"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="34.5" customHeight="1">
@@ -32652,7 +32827,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="98"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="39" customHeight="1">
@@ -32663,44 +32838,37 @@
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="98"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="45" customHeight="1">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:7" ht="76.8" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="102" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" customHeight="1">
-      <c r="A7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="F6" s="100" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32714,16 +32882,16 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32740,18 +32908,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30.75" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -32760,7 +32928,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>9</v>
@@ -32777,7 +32945,7 @@
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -32797,16 +32965,16 @@
     </row>
     <row r="4" spans="1:8" ht="32.25" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>9</v>
@@ -32815,7 +32983,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>13</v>
@@ -32823,21 +32991,33 @@
     </row>
     <row r="5" spans="1:8" ht="33.75" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -32851,7 +33031,7 @@
     </row>
     <row r="7" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -32880,16 +33060,16 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -32906,18 +33086,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="36" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -32926,7 +33106,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>9</v>
@@ -32943,95 +33123,111 @@
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.15" customHeight="1">
+    <row r="4" spans="1:8" ht="43.2" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.15" customHeight="1">
+    <row r="5" spans="1:8" ht="409.2" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="32.25" customHeight="1">
+        <v>52</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="69" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>146</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="F6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -33064,14 +33260,14 @@
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="49.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -33088,18 +33284,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4">
       <c r="A2" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -33119,7 +33315,7 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -33133,7 +33329,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -33147,7 +33343,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -33161,7 +33357,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -33175,7 +33371,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -33208,13 +33404,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="49.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -33231,18 +33427,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4">
       <c r="A2" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -33262,7 +33458,7 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -33276,7 +33472,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -33290,7 +33486,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -33304,7 +33500,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -33318,7 +33514,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -33345,17 +33541,17 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" customWidth="1"/>
-    <col min="5" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="64.44140625" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1">
@@ -33375,48 +33571,48 @@
         <v>4</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="25.5" customHeight="1">
       <c r="A2" s="73" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="75" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="71"/>
       <c r="F2" s="71"/>
       <c r="G2" s="71"/>
       <c r="H2" s="72"/>
       <c r="I2" s="60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="37.5" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>16</v>
@@ -33431,7 +33627,7 @@
     </row>
     <row r="4" spans="1:9" ht="37.5" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>13</v>
@@ -33452,35 +33648,35 @@
     </row>
     <row r="5" spans="1:9" ht="37.5" customHeight="1">
       <c r="A5" s="76" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="76"/>
       <c r="D5" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
       <c r="G5" s="65"/>
       <c r="H5" s="66"/>
       <c r="I5" s="60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="37.5" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>50</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>9</v>
@@ -33489,7 +33685,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>10</v>
@@ -33498,33 +33694,33 @@
     </row>
     <row r="7" spans="1:9" ht="37.5" customHeight="1">
       <c r="A7" s="89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
       <c r="D7" s="90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="90"/>
       <c r="F7" s="90"/>
       <c r="G7" s="90"/>
       <c r="H7" s="91"/>
       <c r="I7" s="60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="86.45" customHeight="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="86.4" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="26" t="s">
         <v>9</v>
@@ -33533,25 +33729,25 @@
         <v>13</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="60"/>
     </row>
-    <row r="9" spans="1:9" ht="49.9" customHeight="1">
+    <row r="9" spans="1:9" ht="49.95" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>9</v>
@@ -33560,7 +33756,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>18</v>
@@ -33569,16 +33765,16 @@
     </row>
     <row r="10" spans="1:9" ht="60.6" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>9</v>
@@ -33587,7 +33783,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>18</v>
@@ -33596,16 +33792,16 @@
     </row>
     <row r="11" spans="1:9" ht="72" customHeight="1">
       <c r="A11" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="26" t="s">
         <v>9</v>
@@ -33614,25 +33810,25 @@
         <v>13</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="60"/>
     </row>
-    <row r="12" spans="1:9" ht="45">
+    <row r="12" spans="1:9" ht="43.2">
       <c r="A12" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>9</v>
@@ -33641,16 +33837,16 @@
         <v>13</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>18</v>
       </c>
       <c r="I12" s="60"/>
     </row>
-    <row r="13" spans="1:9" ht="28.15" customHeight="1">
+    <row r="13" spans="1:9" ht="28.2" customHeight="1">
       <c r="A13" s="89" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="90"/>
       <c r="C13" s="90"/>
@@ -33660,21 +33856,21 @@
       <c r="G13" s="90"/>
       <c r="H13" s="91"/>
       <c r="I13" s="60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.8">
       <c r="A14" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="C14" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>100</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>101</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>9</v>
@@ -33683,7 +33879,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>13</v>
@@ -33692,7 +33888,7 @@
     </row>
     <row r="15" spans="1:9" ht="33" customHeight="1">
       <c r="A15" s="89" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" s="90"/>
       <c r="C15" s="90"/>
@@ -33703,74 +33899,113 @@
       <c r="H15" s="91"/>
       <c r="I15" s="60"/>
     </row>
-    <row r="16" spans="1:9" ht="28.15" customHeight="1">
+    <row r="16" spans="1:9" ht="28.2" customHeight="1">
       <c r="A16" s="50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="60"/>
+    </row>
+    <row r="17" spans="1:9" ht="31.2" customHeight="1">
+      <c r="A17" s="89" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="60"/>
-    </row>
-    <row r="17" spans="5:7" ht="14.25" customHeight="1">
-      <c r="E17" s="10"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="5:7" ht="14.25" customHeight="1">
-      <c r="E18" s="10"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="5:7" ht="14.25" customHeight="1">
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="41.4" customHeight="1">
+      <c r="A18" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="60"/>
+    </row>
+    <row r="19" spans="1:9" ht="14.25" customHeight="1">
       <c r="E19" s="10"/>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="5:7" ht="14.25" customHeight="1">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1">
       <c r="E20" s="10"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="5:7" ht="14.25" customHeight="1">
+    <row r="21" spans="1:9" ht="14.25" customHeight="1">
       <c r="E21" s="10"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="5:7" ht="14.25" customHeight="1">
+    <row r="22" spans="1:9" ht="14.25" customHeight="1">
       <c r="E22" s="10"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="5:7" ht="14.25" customHeight="1">
+    <row r="23" spans="1:9" ht="14.25" customHeight="1">
       <c r="E23" s="10"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="5:7" ht="14.25" customHeight="1">
+    <row r="24" spans="1:9" ht="14.25" customHeight="1">
       <c r="E24" s="10"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="5:7" ht="14.25" customHeight="1">
+    <row r="25" spans="1:9" ht="14.25" customHeight="1">
       <c r="E25" s="10"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="5:7" ht="14.25" customHeight="1">
+    <row r="26" spans="1:9" ht="14.25" customHeight="1">
       <c r="E26" s="10"/>
       <c r="G26" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26" xr:uid="{00000000-0002-0000-0800-000000000000}">

</xml_diff>

<commit_message>
review on ashry edits in SRS.
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C4BC19-2F2C-4B2F-AE66-171E199D6FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAB2808-723F-4EB1-9C2C-21501396053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="9420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="163">
   <si>
     <t>Review No.</t>
   </si>
@@ -568,6 +566,16 @@
   <si>
     <t>1-The impact summary needs to be clarified.
 2-Add more than one solution like postponed to the next release</t>
+  </si>
+  <si>
+    <t>Version 2.0</t>
+  </si>
+  <si>
+    <t>SRS_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update product features and product perspective in administrator.
+</t>
   </si>
 </sst>
 </file>
@@ -1609,7 +1617,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1730,7 +1738,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ar-EG"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2702,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3130,13 +3138,41 @@
       </c>
       <c r="I18" s="60"/>
     </row>
-    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="10"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="10"/>
-      <c r="G20" s="11"/>
+    <row r="19" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="95" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="96"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="60"/>
     </row>
     <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E21" s="10"/>
@@ -3163,11 +3199,12 @@
       <c r="G26" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A19:H19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26" xr:uid="{00000000-0002-0000-0800-000000000000}">
@@ -33412,7 +33449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C639E5-DB13-4402-A4D9-DAAD93882ACC}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -33917,7 +33954,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="C30" sqref="B29:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
review sheet is updated
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAB2808-723F-4EB1-9C2C-21501396053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E8D91B-7124-46AE-A7AD-4A2F74E214E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="9420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="188">
   <si>
     <t>Review No.</t>
   </si>
@@ -577,6 +579,81 @@
     <t xml:space="preserve">Update product features and product perspective in administrator.
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">the 8 character text are in which language /is user able to enter in arabic language </t>
+  </si>
+  <si>
+    <t>"It can be a combination of numbers and some special characters _, # " are those only the accepted characters ?</t>
+  </si>
+  <si>
+    <t>11 numbers in which format / according to which country // should state that it should start with "01"</t>
+  </si>
+  <si>
+    <t>is this unique UID is visable to the user ?</t>
+  </si>
+  <si>
+    <t>what is the content of the confirmation message?</t>
+  </si>
+  <si>
+    <t>how is it going to search the admin table if no data is entered /should refer to that admin must enter username and password field first?</t>
+  </si>
+  <si>
+    <t>"a button (add trip) and submit button" what is the diffrence?</t>
+  </si>
+  <si>
+    <t>what is the curency ?</t>
+  </si>
+  <si>
+    <t>"Dates should be written by the user and should start from the day it’s recorded" is user able to add tour ? // if is the admin what is meant by recoreded</t>
+  </si>
+  <si>
+    <t>is admin able to add images from add image button ??</t>
+  </si>
+  <si>
+    <t>what is the admin add the same image 2 time ??</t>
+  </si>
+  <si>
+    <t>osama</t>
+  </si>
+  <si>
+    <t>17/6</t>
+  </si>
+  <si>
+    <t>17/7</t>
+  </si>
+  <si>
+    <t>17/8</t>
+  </si>
+  <si>
+    <t>17/9</t>
+  </si>
+  <si>
+    <t>17/10</t>
+  </si>
+  <si>
+    <t>17/11</t>
+  </si>
+  <si>
+    <t>17/12</t>
+  </si>
+  <si>
+    <t>17/13</t>
+  </si>
+  <si>
+    <t>17/14</t>
+  </si>
+  <si>
+    <t>17/15</t>
+  </si>
+  <si>
+    <t>17/16</t>
+  </si>
+  <si>
+    <t>19/5</t>
+  </si>
+  <si>
+    <t>Version 2.1</t>
+  </si>
 </sst>
 </file>
 
@@ -585,7 +662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,6 +743,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1617,7 +1700,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1738,7 +1821,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ar-EG"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2708,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3169,45 +3252,260 @@
       <c r="E20" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="62"/>
+      <c r="F20" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>153</v>
+      </c>
       <c r="H20" s="63"/>
       <c r="I20" s="60"/>
     </row>
-    <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="10"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="10"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="10"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="10"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="10"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="10"/>
-      <c r="G26" s="11"/>
+    <row r="21" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="95" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="96"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="60"/>
+    </row>
+    <row r="22" spans="1:9" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B25" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B28" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B29" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B32" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="G32" s="56" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A19:H19"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E26" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4 E6:E32" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fixing bugs and update naming convention of bug report with adding bug review to review sheet
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E6B8F4-D2E6-424B-BE87-5F74830A70CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00FD514-5BC4-404E-8F80-BC93A4BC748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="196">
   <si>
     <t>Review No.</t>
   </si>
@@ -664,6 +664,18 @@
   </si>
   <si>
     <t>Login Admin Page Test cases steps &amp; Precondtions not not described correctly for example in steps you check the box after clicking login button</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_User_Sign_Up_007 not correct according REQ-07-Signup in SRS and same in bug report</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>TC_User_Sign_Up_008 not correct according REQ-07-Signup in SRS and same in bug report</t>
   </si>
 </sst>
 </file>
@@ -2116,7 +2128,7 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -32735,7 +32747,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32824,9 +32836,7 @@
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
-      <c r="E4" s="47" t="s">
-        <v>9</v>
-      </c>
+      <c r="E4" s="47"/>
       <c r="F4" s="25"/>
       <c r="G4" s="35"/>
       <c r="H4" s="35"/>
@@ -33249,15 +33259,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ACC88D-AEC9-45BB-8F2C-785C83602618}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -33300,13 +33311,17 @@
         <v>190</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="G2" s="35">
+        <v>44705</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -33322,27 +33337,73 @@
         <v>191</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="49"/>
+      <c r="G3" s="35">
+        <v>44705</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="48">
+        <v>44706</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="35">
+        <v>44706</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="48">
+        <v>44706</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="35">
+        <v>44706</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{43EE605C-4A86-413C-81B4-433FFE0F9D6A}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{43EE605C-4A86-413C-81B4-433FFE0F9D6A}">
       <formula1>Options</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Project Schedule for delviery
</commit_message>
<xml_diff>
--- a/Monitor and Control/Reviews.xlsx
+++ b/Monitor and Control/Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA2CE3F-F7E8-4CDD-92D2-8FAA388203D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6865BA68-A143-492B-8698-E857C09E0F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="13" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="198">
   <si>
     <t>Review No.</t>
   </si>
@@ -667,6 +667,24 @@
   </si>
   <si>
     <t>Version 1.7</t>
+  </si>
+  <si>
+    <t>TP_01</t>
+  </si>
+  <si>
+    <t>25/5</t>
+  </si>
+  <si>
+    <t>There are no tests include exploartory testing, please remove it from the plan in section validation.</t>
+  </si>
+  <si>
+    <t>26/5</t>
+  </si>
+  <si>
+    <t>No issues found.</t>
+  </si>
+  <si>
+    <t>BR_01</t>
   </si>
 </sst>
 </file>
@@ -1580,9 +1598,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1599,6 +1614,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3192,7 +3210,7 @@
       <c r="E7" s="109"/>
       <c r="F7" s="109"/>
       <c r="G7" s="109"/>
-      <c r="H7" s="110"/>
+      <c r="H7" s="116"/>
       <c r="I7" s="60" t="s">
         <v>103</v>
       </c>
@@ -3342,7 +3360,7 @@
       <c r="E13" s="109"/>
       <c r="F13" s="109"/>
       <c r="G13" s="109"/>
-      <c r="H13" s="110"/>
+      <c r="H13" s="116"/>
       <c r="I13" s="60" t="s">
         <v>103</v>
       </c>
@@ -3384,7 +3402,7 @@
       <c r="E15" s="109"/>
       <c r="F15" s="109"/>
       <c r="G15" s="109"/>
-      <c r="H15" s="110"/>
+      <c r="H15" s="116"/>
       <c r="I15" s="60"/>
     </row>
     <row r="16" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3424,7 +3442,7 @@
       <c r="E17" s="109"/>
       <c r="F17" s="109"/>
       <c r="G17" s="109"/>
-      <c r="H17" s="110"/>
+      <c r="H17" s="116"/>
       <c r="I17" s="60" t="s">
         <v>103</v>
       </c>
@@ -3466,7 +3484,7 @@
       <c r="E19" s="109"/>
       <c r="F19" s="109"/>
       <c r="G19" s="109"/>
-      <c r="H19" s="110"/>
+      <c r="H19" s="116"/>
       <c r="I19" s="60" t="s">
         <v>103</v>
       </c>
@@ -3506,7 +3524,7 @@
       <c r="E21" s="109"/>
       <c r="F21" s="109"/>
       <c r="G21" s="109"/>
-      <c r="H21" s="110"/>
+      <c r="H21" s="116"/>
       <c r="I21" s="60"/>
     </row>
     <row r="22" spans="1:9" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3730,17 +3748,17 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111" t="s">
+      <c r="A33" s="110" t="s">
         <v>187</v>
       </c>
-      <c r="B33" s="112"/>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="111" t="s">
+      <c r="B33" s="111"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="112"/>
+      <c r="I33" s="110" t="s">
         <v>188</v>
       </c>
       <c r="J33" s="92"/>
@@ -3754,15 +3772,15 @@
       <c r="R33" s="109"/>
     </row>
     <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114"/>
-      <c r="B34" s="115"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="114"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="113"/>
       <c r="J34" s="92"/>
       <c r="K34" s="92"/>
       <c r="L34" s="92"/>
@@ -3775,16 +3793,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A19:H19"/>
     <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q34:R34"/>
     <mergeCell ref="A33:H34"/>
     <mergeCell ref="I33:I34"/>
     <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A19:H19"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="1">
@@ -33449,7 +33467,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33650,14 +33668,81 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87AEFF5-F675-4891-84E9-A6014F4FDE3F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="35">
+        <v>44706</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{F9998060-3CA5-4CA1-9721-57E8848EB83C}">
+      <formula1>Options</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -33814,28 +33899,135 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF38150-4F6D-490D-AB31-ACE32D43D5BA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="38.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{54877E34-370C-4F23-B6F9-8DC9D3862CB0}">
+      <formula1>Options</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E7D7A4-F2C8-448C-B10A-90DB438F1637}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="29.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2" xr:uid="{9F53CF53-7C0D-4147-9C6F-2316339E4119}">
+      <formula1>Options</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>